<commit_message>
Updated interface with audio feedback
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -12,12 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>Exercise</t>
   </si>
   <si>
     <t>Angle</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
   <si>
     <t>Commentary</t>
@@ -35,6 +38,129 @@
 Then return to the starting position, and you can repeat this movement 5 times.</t>
   </si>
   <si>
+    <t>BBRW</t>
+  </si>
+  <si>
+    <t>BRGM</t>
+  </si>
+  <si>
+    <t>BRK4</t>
+  </si>
+  <si>
+    <t>BRKZ</t>
+  </si>
+  <si>
+    <t>BULG</t>
+  </si>
+  <si>
+    <t>CHOP</t>
+  </si>
+  <si>
+    <t>CLMB</t>
+  </si>
+  <si>
+    <t>FRLG</t>
+  </si>
+  <si>
+    <t>GLUT</t>
+  </si>
+  <si>
+    <t>HMST</t>
+  </si>
+  <si>
+    <t>HMSZ</t>
+  </si>
+  <si>
+    <t>HSSE</t>
+  </si>
+  <si>
+    <t>IPST</t>
+  </si>
+  <si>
+    <t>JPJK</t>
+  </si>
+  <si>
+    <t>LGST</t>
+  </si>
+  <si>
+    <t>LPLT</t>
+  </si>
+  <si>
+    <t>LTDB</t>
+  </si>
+  <si>
+    <t>LTLG</t>
+  </si>
+  <si>
+    <t>LTLP</t>
+  </si>
+  <si>
+    <t>LTPL</t>
+  </si>
+  <si>
+    <t>MOZR</t>
+  </si>
+  <si>
+    <t>OLDL</t>
+  </si>
+  <si>
+    <t>PLCI</t>
+  </si>
+  <si>
+    <t>PLLU</t>
+  </si>
+  <si>
+    <t>PLM1</t>
+  </si>
+  <si>
+    <t>PLTO</t>
+  </si>
+  <si>
+    <t>PUSH</t>
+  </si>
+  <si>
+    <t>RFSN</t>
+  </si>
+  <si>
+    <t>SKIS</t>
+  </si>
+  <si>
+    <t>SKJP</t>
+  </si>
+  <si>
+    <t>SMSQ</t>
+  </si>
+  <si>
+    <t>SQOC</t>
+  </si>
+  <si>
+    <t>SQUA</t>
+  </si>
+  <si>
+    <t>STRZ</t>
+  </si>
+  <si>
+    <t>TRID</t>
+  </si>
+  <si>
+    <t>TRST</t>
+  </si>
+  <si>
+    <t>YMWS</t>
+  </si>
+  <si>
+    <t>YPST</t>
+  </si>
+  <si>
+    <t>right_elbow</t>
+  </si>
+  <si>
+    <t>Starting position standing, feet hip-width apart, arms extended in a Y form, side bends to one side and to the other until whole side of body is stretched, with a 5 second hold. 3 repetitions on each side.</t>
+  </si>
+  <si>
+    <t>ZRCS</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
@@ -57,9 +183,6 @@
   </si>
   <si>
     <t>left_knee</t>
-  </si>
-  <si>
-    <t>right_elbow</t>
   </si>
   <si>
     <t>left_elbow</t>
@@ -128,13 +251,18 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <bottom style="thin">
+        <color rgb="FFD2D2DF"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -146,6 +274,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -370,7 +501,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="78.13"/>
+    <col customWidth="1" min="3" max="3" width="9.88"/>
+    <col customWidth="1" min="4" max="4" width="77.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -380,20 +512,276 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
+      <c r="A2" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="1">
+        <v>180.0</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42">
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43">
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44">
+      <c r="F44" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -412,300 +800,300 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
         <v>23.0</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>25.0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>27.0</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>12.0</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="5">
         <v>13.0</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5">
         <v>14.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="4">
+        <v>55</v>
+      </c>
+      <c r="B3" s="5">
         <v>24.0</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>26.0</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>28.0</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>9.0</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>10.0</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <v>11.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="4">
+        <v>45</v>
+      </c>
+      <c r="B4" s="5">
         <v>15.0</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>13.0</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <v>11.0</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
         <v>7.0</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <v>6.0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="5">
         <v>5.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="4">
+        <v>56</v>
+      </c>
+      <c r="B5" s="5">
         <v>16.0</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>14.0</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>12.0</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>4.0</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>3.0</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="5">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4">
+        <v>57</v>
+      </c>
+      <c r="B6" s="5">
         <v>12.0</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>24.0</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <v>26.0</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
         <v>5.0</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <v>12.0</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="5">
         <v>13.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4">
+        <v>58</v>
+      </c>
+      <c r="B7" s="5">
         <v>11.0</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>23.0</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>25.0</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="5">
         <v>2.0</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="5">
         <v>9.0</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="5">
         <v>10.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="4">
+        <v>59</v>
+      </c>
+      <c r="B8" s="5">
         <v>32.0</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>28.0</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <v>26.0</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="5">
         <v>20.0</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="5">
         <v>21.0</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="5">
         <v>13.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="4">
+        <v>60</v>
+      </c>
+      <c r="B9" s="5">
         <v>31.0</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>27.0</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <v>25.0</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="5">
         <v>23.0</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="5">
         <v>24.0</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="5">
         <v>10.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="4">
+        <v>61</v>
+      </c>
+      <c r="B10" s="5">
         <v>14.0</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <v>12.0</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="5">
         <v>24.0</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="5">
         <v>6.0</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="5">
         <v>5.0</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="5">
         <v>12.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="4">
+        <v>62</v>
+      </c>
+      <c r="B11" s="5">
         <v>13.0</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <v>11.0</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="5">
         <v>23.0</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="5">
         <v>3.0</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="5">
         <v>2.0</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="5">
         <v>9.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="4">
+        <v>63</v>
+      </c>
+      <c r="B12" s="5">
         <v>0.0</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <v>33.0</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="5">
         <v>12.0</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="5">
         <v>0.0</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="5">
         <v>1.0</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="5">
         <v>5.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="4">
+        <v>64</v>
+      </c>
+      <c r="B13" s="5">
         <v>0.0</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="5">
         <v>33.0</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="5">
         <v>11.0</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="5">
         <v>0.0</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="5">
         <v>1.0</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="5">
         <v>2.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated interface with new audio feedback
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
   <si>
     <t>Exercise</t>
   </si>
@@ -23,7 +23,10 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Commentary</t>
+    <t>Short Commentary</t>
+  </si>
+  <si>
+    <t>Long commentary</t>
   </si>
   <si>
     <t>1LBR</t>
@@ -32,133 +35,253 @@
     <t>right_knee</t>
   </si>
   <si>
-    <t>For this exercise, lie on your back, place your arms flat alongside your body and then bend your knees. 
-Raise your right knee to 90 degrees: You're in the starting position.
-Now raise your pelvis with your left leg so that your left shoulder, hip and knee form a straight line.
-Then return to the starting position, and you can repeat this movement 5 times.</t>
+    <t>Lying on your back- knees bent, feet on the mat, perform a bridge lift. At the same time, lift one leg into the air. Alternate sides-repeat 5 times on each side.</t>
+  </si>
+  <si>
+    <t>More information to come</t>
   </si>
   <si>
     <t>BBRW</t>
   </si>
   <si>
+    <t>Standing, knees slightly bent, torso flexed, pull the dumbbell towards your body.Repeat 10 times.</t>
+  </si>
+  <si>
     <t>BRGM</t>
   </si>
   <si>
+    <t>Lying on your back, with your legs extended and supported by the ball, perform the lift into the plank, Upper arms and shoulder blades remaining in contact with the mat. Repeat 10 times.</t>
+  </si>
+  <si>
     <t>BRK4</t>
   </si>
   <si>
+    <t>On all fours on the mat, alternate uplifting the opposite lower and upper limb simultaneously. 5 repetitions on each side.</t>
+  </si>
+  <si>
     <t>BRKZ</t>
   </si>
   <si>
+    <t xml:space="preserve">Lying on your back, lay the opposite limbs toward mat simultaneously, strengthen Your abdomen. Repeat 10 time. </t>
+  </si>
+  <si>
     <t>BULG</t>
   </si>
   <si>
+    <t>Standing on one leg and with the other supported by a chair behind you, perform squats on one leg. The knee of the standing leg should not exceed the line of the thumb.</t>
+  </si>
+  <si>
     <t>CHOP</t>
   </si>
   <si>
+    <t>In a 4-point stance, rotate sideways following the extended upper limb- open the chest, head rotating towards the upper limb. Hold a while. Come back by tucking the upper limb under the other, until shoulder touches the mat. In the extreme positions, hold for 5 seconds. Repeat 3 times on each side.</t>
+  </si>
+  <si>
     <t>CLMB</t>
   </si>
   <si>
+    <t>In the plank, alternate pulling the knees towards the shoulders, with the knees pointing straight below the chest at the maximum range of motion. Repeat 5 times on each side.</t>
+  </si>
+  <si>
     <t>FRLG</t>
   </si>
   <si>
+    <t>Perform a frontal lunge, back leg knee is going close to the mat. Repeat 5 times for each side.</t>
+  </si>
+  <si>
     <t>GLUT</t>
   </si>
   <si>
+    <t>On all fours- lift Your one leg up, with knee in flexion- alternate lower limbs- 10 reps on each leg</t>
+  </si>
+  <si>
+    <t>HLTC</t>
+  </si>
+  <si>
+    <t>From standing on the box, lower one leg down off the box, using the knee bend of the standing leg. Touch the heel to the mat, alternate limbs, repeat 5 times, each side.</t>
+  </si>
+  <si>
     <t>HMST</t>
   </si>
   <si>
+    <t>Laying on Your back, using theraband, lift one extended leg for hamstring stretch. Hold position for 10 seconds, repeat 5 times.</t>
+  </si>
+  <si>
     <t>HMSZ</t>
   </si>
   <si>
+    <t>Sitting on a chair, perform a stretch of the extended lower limb using a theraband, the theraband is around the foot, pulling the toe in, at the same time as pulling the straighten torso towards the toe. Duration in final position- 20 seconds. Repeat on other leg.</t>
+  </si>
+  <si>
     <t>HSSE</t>
   </si>
   <si>
+    <t xml:space="preserve">Lying on your back, lay the opposite limbs toward mat simultaneously, while holding the ball,strengthen Your abdomen. Repeat 10 time. </t>
+  </si>
+  <si>
     <t>IPST</t>
   </si>
   <si>
+    <t>From kneeling position, with one leg stepped forward, perform a groin stretch, by leaning Your pelvis forward. Hold for 10 seconds. repeat 5 times.</t>
+  </si>
+  <si>
     <t>JPJK</t>
   </si>
   <si>
+    <t>Perform jumping jacks, with straightened arms. Repeat 10 times.</t>
+  </si>
+  <si>
     <t>LGST</t>
   </si>
   <si>
-    <t>LPLT</t>
+    <t>Perform a groin (hip flexor) stretch in the kneeling position, with one lower limb in front step. To stretch the back of the thighs, shift weight to the back, keeping the front lower limb extended, pull the toe in. Duration 20 seconds each time. Repeat 2 times on each side.</t>
   </si>
   <si>
     <t>LTDB</t>
   </si>
   <si>
+    <t>Lying on your stomach, arms upright, move your arms down to body, while holding your elbows close to trunk, repeat 10 times, head resting on forehead.</t>
+  </si>
+  <si>
     <t>LTLG</t>
   </si>
   <si>
-    <t>LTLP</t>
+    <t>Slowly transfer weight between sideway lunges, with feets on the mat, torso remains straighten. repeat 5 times at each side.</t>
   </si>
   <si>
     <t>LTPL</t>
   </si>
   <si>
+    <t>Perform a lateral plank. The whole body is facing forward. Head in extension of the spine. Free upper limb extended in the air. Hold for 10 seconds, repeat 3 times on each side.</t>
+  </si>
+  <si>
+    <t>MOZH</t>
+  </si>
+  <si>
+    <t>Sitting on the chair, touch the opposite ankle with your hand, the other upper limb goes up, rotate You chest and look at the upper hand. Repeat 5 times on each side.</t>
+  </si>
+  <si>
     <t>MOZR</t>
   </si>
   <si>
+    <t>Sitting on a chair,with your arms crossed on your shoulders, perform a trunk rotation, head is copying the trunk. Repeat 5 times on each side.</t>
+  </si>
+  <si>
     <t>OLDL</t>
   </si>
   <si>
+    <t>From standing, lean torso down at the same time as one extended leg descends, extend back to standing with weight in one hand. Repeat 10 times.</t>
+  </si>
+  <si>
     <t>PLCI</t>
   </si>
   <si>
-    <t>PLLU</t>
+    <t>In a plank, with both forearms resting on the ball, perform small circles with the ball. Keep torso extended. 5 circles each side.</t>
   </si>
   <si>
     <t>PLM1</t>
   </si>
   <si>
+    <t>In a ball plank, with forearm support, knees straight, lower knees to the mat, knees not touching the ground, ball may roll out of place.Repeat 10 times</t>
+  </si>
+  <si>
     <t>PLTO</t>
   </si>
   <si>
+    <t>In the plank, alternate touching the opposite shoulder with one hand. keeping the trunk and head in same position. Repeat 5 times each side.</t>
+  </si>
+  <si>
     <t>PUSH</t>
   </si>
   <si>
+    <t>Perform a push-up, torso remains rigid, head in extension of spine. Variation with knee support.</t>
+  </si>
+  <si>
     <t>RFSN</t>
   </si>
   <si>
+    <t>Change yoga positions from roof to cobra, hold in for 3-5 seconds, repeat 5 times each.</t>
+  </si>
+  <si>
     <t>SKIS</t>
   </si>
   <si>
+    <t>From a standing position on bent lower legs, perform a sideways jump on both lower legs at once- stabilize in knee flexion, knees facing forward. Repeat 5 times on each side.</t>
+  </si>
+  <si>
     <t>SKJP</t>
   </si>
   <si>
+    <t>From standing on one leg,knee slightly bent, jump to the other leg, knees always facing forward on the rebound. Stabilize the position and jump to the other leg. Repeat 10 times.</t>
+  </si>
+  <si>
     <t>SMSQ</t>
   </si>
   <si>
+    <t>Perform a wide squat, with weight in the middle, knees going into an outward bend, pelvis dropping to knee level. Hold for 15 seconds, repeat 5 times.</t>
+  </si>
+  <si>
     <t>SQOC</t>
   </si>
   <si>
+    <t>From standing barefoot at two balance trainers,  pelvic width, perform a squat. Knees point forward and do not exceed the edge of the thumbs. Repeat 10 times</t>
+  </si>
+  <si>
     <t>SQUA</t>
   </si>
   <si>
+    <t>Perform a squat, knees facing forward, not going over the edge of the leg.Repeat 10 times</t>
+  </si>
+  <si>
+    <t>STAR</t>
+  </si>
+  <si>
+    <t>From a standing position, touch all 7 points on the mat with one foot</t>
+  </si>
+  <si>
+    <t>STDZ</t>
+  </si>
+  <si>
+    <t>From standing at pelvic width, drop to sitting on a chair, knees facing forward, torso braced, buttocks touching the chair, no weight transfer, torso may lean slightly forward, then return to standing. Repeat 5 times.</t>
+  </si>
+  <si>
     <t>STRZ</t>
   </si>
   <si>
+    <t>Sitting on a chair, one lower leg in front of the body, the other next to the chair, use a theraband to stretch the front  thigh muscles, pulling the heel of back foot towards the buttocks.</t>
+  </si>
+  <si>
     <t>TRID</t>
   </si>
   <si>
+    <t>Supported by your hands on the box behind you, lower your body down to about a 90-degree bend at the elbows.  The lower limbs may be extended or bent at the knees. Repeat 10 times</t>
+  </si>
+  <si>
     <t>TRST</t>
   </si>
   <si>
+    <t>Standing , using the upper limb, perform a trapezius extension by tilting the head to the side. The other upper limb stays close to the body, wrist bent upwards. Repeat 2 times each side, hold for 15s.</t>
+  </si>
+  <si>
     <t>YMWS</t>
   </si>
   <si>
+    <t>While standing, perform 3 positions of upper limb - erect overhead in a Y shape, sideways with elbows at shoulder level, transitioning to pulling elbows to torso, moving by engaging and retracting shoulder blades. Return to the starting position. Repeat 8 times.</t>
+  </si>
+  <si>
     <t>YPST</t>
   </si>
   <si>
     <t>right_elbow</t>
   </si>
   <si>
-    <t>Starting position standing, feet hip-width apart, arms extended in a Y form, side bends to one side and to the other until whole side of body is stretched, with a 5 second hold. 3 repetitions on each side.</t>
+    <t>From standing, arms straighten in Y position, bend to sides, to maximal range, for stretching side of your trunk,hold for 3 seconds, repeat 5 times</t>
   </si>
   <si>
     <t>ZRCS</t>
+  </si>
+  <si>
+    <t>Sitting on a chair, with your elbows close to your body, perform a theraband extension, arms going out to the side and extending the theraband, elbows staying close to your body. Repeat 10 times.</t>
   </si>
   <si>
     <t>name</t>
@@ -216,7 +339,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -236,6 +359,11 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -251,10 +379,47 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border/>
     <border>
-      <bottom style="thin">
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD2D2DF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD2D2DF"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
         <color rgb="FFD2D2DF"/>
       </bottom>
     </border>
@@ -262,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -275,8 +440,26 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -503,6 +686,7 @@
   <cols>
     <col customWidth="1" min="3" max="3" width="9.88"/>
     <col customWidth="1" min="4" max="4" width="77.25"/>
+    <col customWidth="1" min="5" max="5" width="16.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -518,263 +702,389 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
         <v>90.0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>16</v>
+      <c r="A12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>18</v>
+        <v>31</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>39</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="F18" s="3"/>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>41</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="F19" s="3"/>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="F20" s="3"/>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>45</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="F21" s="3"/>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
-        <v>26</v>
+      <c r="A22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="F22" s="3"/>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>49</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="F23" s="3"/>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="F24" s="3"/>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>29</v>
+        <v>53</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="F25" s="3"/>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>30</v>
+        <v>55</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="F26" s="3"/>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>31</v>
+        <v>57</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="F27" s="3"/>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="F28" s="3"/>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>33</v>
+        <v>61</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="F29" s="3"/>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>34</v>
+        <v>63</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="F30" s="3"/>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>35</v>
+        <v>65</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="F31" s="3"/>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>36</v>
+        <v>67</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="F32" s="3"/>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>37</v>
+        <v>69</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="F33" s="3"/>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>38</v>
+        <v>71</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="F34" s="3"/>
     </row>
     <row r="35">
-      <c r="A35" s="3" t="s">
-        <v>39</v>
+      <c r="A35" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="F35" s="3"/>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="s">
-        <v>40</v>
+      <c r="A36" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="F36" s="3"/>
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>41</v>
+        <v>77</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="F37" s="3"/>
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
-        <v>42</v>
+        <v>79</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="F38" s="3"/>
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>43</v>
+        <v>81</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="F39" s="3"/>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="1">
-        <v>180.0</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>46</v>
+        <v>83</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="F40" s="3"/>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>47</v>
+        <v>85</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="1">
+        <v>180.0</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="F41" s="3"/>
     </row>
     <row r="42">
+      <c r="A42" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="F42" s="3"/>
     </row>
     <row r="43">
@@ -782,6 +1092,9 @@
     </row>
     <row r="44">
       <c r="F44" s="3"/>
+    </row>
+    <row r="45">
+      <c r="F45" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -800,300 +1113,300 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5">
+        <v>6</v>
+      </c>
+      <c r="B2" s="11">
         <v>23.0</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="11">
         <v>25.0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="11">
         <v>27.0</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="11">
         <v>12.0</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="11">
         <v>13.0</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="11">
         <v>14.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="5">
+        <v>97</v>
+      </c>
+      <c r="B3" s="11">
         <v>24.0</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="11">
         <v>26.0</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="11">
         <v>28.0</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="11">
         <v>9.0</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="11">
         <v>10.0</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="11">
         <v>11.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="5">
+        <v>86</v>
+      </c>
+      <c r="B4" s="11">
         <v>15.0</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="11">
         <v>13.0</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="11">
         <v>11.0</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="11">
         <v>7.0</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="11">
         <v>6.0</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="11">
         <v>5.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="5">
+        <v>98</v>
+      </c>
+      <c r="B5" s="11">
         <v>16.0</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="11">
         <v>14.0</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="11">
         <v>12.0</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="11">
         <v>4.0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="11">
         <v>3.0</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="11">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="5">
+        <v>99</v>
+      </c>
+      <c r="B6" s="11">
         <v>12.0</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="11">
         <v>24.0</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="11">
         <v>26.0</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="11">
         <v>5.0</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="11">
         <v>12.0</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="11">
         <v>13.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="5">
+        <v>100</v>
+      </c>
+      <c r="B7" s="11">
         <v>11.0</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="11">
         <v>23.0</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="11">
         <v>25.0</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="11">
         <v>2.0</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="11">
         <v>9.0</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="11">
         <v>10.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="5">
+        <v>101</v>
+      </c>
+      <c r="B8" s="11">
         <v>32.0</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="11">
         <v>28.0</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="11">
         <v>26.0</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="11">
         <v>20.0</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="11">
         <v>21.0</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="11">
         <v>13.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="5">
+        <v>102</v>
+      </c>
+      <c r="B9" s="11">
         <v>31.0</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="11">
         <v>27.0</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="11">
         <v>25.0</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="11">
         <v>23.0</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="11">
         <v>24.0</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="11">
         <v>10.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="5">
+        <v>103</v>
+      </c>
+      <c r="B10" s="11">
         <v>14.0</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="11">
         <v>12.0</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="11">
         <v>24.0</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="11">
         <v>6.0</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="11">
         <v>5.0</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="11">
         <v>12.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="5">
+        <v>104</v>
+      </c>
+      <c r="B11" s="11">
         <v>13.0</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="11">
         <v>11.0</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="11">
         <v>23.0</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="11">
         <v>3.0</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="11">
         <v>2.0</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="11">
         <v>9.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="5">
+        <v>105</v>
+      </c>
+      <c r="B12" s="11">
         <v>0.0</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="11">
         <v>33.0</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="11">
         <v>12.0</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="11">
         <v>0.0</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="11">
         <v>1.0</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="11">
         <v>5.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="5">
+        <v>106</v>
+      </c>
+      <c r="B13" s="11">
         <v>0.0</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="11">
         <v>33.0</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="11">
         <v>11.0</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="11">
         <v>0.0</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="11">
         <v>1.0</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="11">
         <v>2.0</v>
       </c>
     </row>

</xml_diff>